<commit_message>
[Doc] Edit dynamo table
</commit_message>
<xml_diff>
--- a/Docs/Thiết kế dynamodb table.xlsx
+++ b/Docs/Thiết kế dynamodb table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DynamoDB Design" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Access Patterns</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>StudentId</t>
+  </si>
+  <si>
+    <t>ScoreboardId</t>
   </si>
 </sst>
 </file>
@@ -353,13 +356,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -371,7 +372,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,24 +661,24 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" customWidth="1"/>
-    <col min="3" max="3" width="58.88671875" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -685,7 +688,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -695,7 +698,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -705,7 +708,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -715,7 +718,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -725,7 +728,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -735,7 +738,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -745,7 +748,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -766,40 +769,40 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -817,11 +820,11 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -841,9 +844,9 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
@@ -861,11 +864,11 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -893,9 +896,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
@@ -921,11 +924,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -945,9 +948,9 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="4" t="s">
         <v>47</v>
       </c>
@@ -965,11 +968,11 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -983,9 +986,9 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
@@ -997,9 +1000,9 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1013,9 +1016,9 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="4" t="s">
         <v>53</v>
       </c>
@@ -1027,11 +1030,11 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1057,9 +1060,9 @@
       </c>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="4" t="s">
         <v>57</v>
       </c>
@@ -1083,11 +1086,11 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1105,9 +1108,9 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="4" t="s">
         <v>61</v>
       </c>
@@ -1123,11 +1126,11 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1145,9 +1148,9 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
@@ -1163,11 +1166,11 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1185,9 +1188,9 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="4" t="s">
         <v>36</v>
       </c>
@@ -1203,9 +1206,9 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1217,15 +1220,17 @@
       <c r="E21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="8"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1235,7 +1240,9 @@
       <c r="E22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1243,16 +1250,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C1:J1"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>

</xml_diff>

<commit_message>
[Doc] Update report file, class & dynamodb diagrams.
</commit_message>
<xml_diff>
--- a/Docs/Thiết kế dynamodb table.xlsx
+++ b/Docs/Thiết kế dynamodb table.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="DynamoDB Design" sheetId="1" r:id="rId1"/>
-    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Access Patterns" sheetId="1" r:id="rId1"/>
+    <sheet name="Multiple Tables Sample" sheetId="3" r:id="rId2"/>
+    <sheet name="Sample Data" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,59 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="122">
   <si>
     <t>Access Patterns</t>
   </si>
   <si>
-    <t>Features</t>
-  </si>
-  <si>
-    <t>Đăng nhập</t>
-  </si>
-  <si>
-    <t>Xem điểm</t>
-  </si>
-  <si>
-    <t>Tìm tài khoản từ tên đăng nhập.</t>
-  </si>
-  <si>
-    <t>Tìm tất cả lớp trong cùng một khối.</t>
-  </si>
-  <si>
-    <t>Tìm tất cả học sinh trong cùng một lớp.</t>
-  </si>
-  <si>
-    <t>Tìm tất cả điểm trong một bảng điểm.</t>
-  </si>
-  <si>
-    <t>Tìm tất cả bảng điểm của một học sinh.</t>
-  </si>
-  <si>
-    <t>Xem điểm, xem lịch học, xem thông tin học sinh</t>
-  </si>
-  <si>
-    <t>Xem điểm, xem thông tin học sinh</t>
-  </si>
-  <si>
-    <t>Nhập điểm</t>
-  </si>
-  <si>
-    <t>Xem lịch dạy</t>
-  </si>
-  <si>
-    <t>Tìm tất cả lịch dạy của một giáo viên.</t>
-  </si>
-  <si>
-    <t>Tìm tất cả lớp có trong lịch dạy của một giáo viên.</t>
-  </si>
-  <si>
-    <t>Xem thông tin giáo viên</t>
-  </si>
-  <si>
-    <t>Tìm thông tin giáo viên từ tài khoản đã đăng nhập.</t>
-  </si>
-  <si>
     <t>Primary Key</t>
   </si>
   <si>
@@ -236,18 +189,224 @@
   </si>
   <si>
     <t>ScoreboardId</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Attritubutes</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Account-Teacher</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Tìm điểm của học sinh</t>
+  </si>
+  <si>
+    <t>Tìm danh sách các lớp đang dạy của giáo viên</t>
+  </si>
+  <si>
+    <t>Tìm tài khoản từ tên đăng nhập</t>
+  </si>
+  <si>
+    <t>Tìm tất cả lớp trong khối</t>
+  </si>
+  <si>
+    <t>Tìm tất cả học sinh trong lớp</t>
+  </si>
+  <si>
+    <t>Tìm lịch dạy của giáo viên</t>
+  </si>
+  <si>
+    <t>Tìm thông tin cá nhân của giáo viên</t>
+  </si>
+  <si>
+    <t>Tìm học sinh theo tên</t>
+  </si>
+  <si>
+    <t>Tìm giáo viên theo tên</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>ScheduleId</t>
+  </si>
+  <si>
+    <t>Schedule01</t>
+  </si>
+  <si>
+    <t>Teacher-Schedule</t>
+  </si>
+  <si>
+    <t>Schedule02</t>
+  </si>
+  <si>
+    <t>Student01</t>
+  </si>
+  <si>
+    <t>Student02</t>
+  </si>
+  <si>
+    <t>Teacher01</t>
+  </si>
+  <si>
+    <t>StudyClass01</t>
+  </si>
+  <si>
+    <t>StudyClass-Schedule</t>
+  </si>
+  <si>
+    <t>StudyClass-Student</t>
+  </si>
+  <si>
+    <t>Student-Scores</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>Scoreboard01</t>
+  </si>
+  <si>
+    <t>ScoreId</t>
+  </si>
+  <si>
+    <t>Score01</t>
+  </si>
+  <si>
+    <t>Score02</t>
+  </si>
+  <si>
+    <t>Scoreboard02</t>
+  </si>
+  <si>
+    <t>Score03</t>
+  </si>
+  <si>
+    <t>Score04</t>
+  </si>
+  <si>
+    <t>Scoreboard03</t>
+  </si>
+  <si>
+    <t>Scoreboard04</t>
+  </si>
+  <si>
+    <t>Score05</t>
+  </si>
+  <si>
+    <t>Score06</t>
+  </si>
+  <si>
+    <t>Score07</t>
+  </si>
+  <si>
+    <t>Score08</t>
+  </si>
+  <si>
+    <t>StudyClassId</t>
+  </si>
+  <si>
+    <t>Grade (GSI-SCS-1-PK)</t>
+  </si>
+  <si>
+    <t>Bảng: "StudyClass-Student", Index: "GSI-SCS-1", PK: grade</t>
+  </si>
+  <si>
+    <t>Bảng: "StudyClass-Student", PK: class id</t>
+  </si>
+  <si>
+    <t>Bảng: "Student-Scores", PK: student id</t>
+  </si>
+  <si>
+    <t>Bảng: "StudyClass-Student", PK: class id, SK: student id</t>
+  </si>
+  <si>
+    <t>Tìm thông tin học sinh</t>
+  </si>
+  <si>
+    <t>Tìm lịch học của một lớp</t>
+  </si>
+  <si>
+    <t>Bảng: "StudyClass-Schedule", PK: class id</t>
+  </si>
+  <si>
+    <t>Bảng: "Teacher-Schedule", PK: teacher id</t>
+  </si>
+  <si>
+    <t>Bảng: "StudyClass-Student", PK: study class id</t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>Bảng: "Account-Teacher", PK: username</t>
+  </si>
+  <si>
+    <t>Bảng: "Account-Teacher", PK: username, SK: teacher id</t>
+  </si>
+  <si>
+    <t>Name (GSI-SCS-2-PK)</t>
+  </si>
+  <si>
+    <t>Bảng: "StudyClass-Student", Index: "GSI-SCS-2", PK: student name</t>
+  </si>
+  <si>
+    <t>Name (GSI-AT-1-PK)</t>
+  </si>
+  <si>
+    <t>Bảng: "Account-Teacher", Index: "GSI-AT-1", PK: teacher name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -278,7 +437,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,13 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,9 +524,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,108 +839,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="58.85546875" customWidth="1"/>
+    <col min="1" max="1" width="45.5546875" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -766,51 +965,1055 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="A21:A40"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:J2"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -820,163 +2023,163 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>27</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>32</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>48</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -986,11 +2189,11 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1000,13 +2203,13 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
-        <v>52</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1016,11 +2219,11 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1030,77 +2233,77 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>55</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>58</v>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1108,17 +2311,17 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1126,21 +2329,21 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>63</v>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1148,17 +2351,17 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1166,21 +2369,21 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>67</v>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1188,17 +2391,17 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="7"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D20" s="4">
         <v>8</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1206,42 +2409,42 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="7" t="s">
-        <v>69</v>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="7"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D22" s="4">
         <v>9</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1250,11 +2453,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B16"/>
@@ -1270,6 +2468,11 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>